<commit_message>
Did code.js: replaceMethod, replaceType, replaceProperty.
</commit_message>
<xml_diff>
--- a/finish code.xlsx
+++ b/finish code.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geral_000\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TG\TGv1000\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,9 +32,6 @@
     <t>wire up client methods to update Type and Method;</t>
   </si>
   <si>
-    <t>write code methods for same;</t>
-  </si>
-  <si>
     <t>change method XML and JavaScript generators to handle Method type and params;</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
     <t>self.renameEvent</t>
   </si>
   <si>
-    <t>self.isReferencedInWorkspace</t>
-  </si>
-  <si>
     <t>Check out (in code.js) self.renameTypeInActiveComic and self.renameMethodInActiveType to be sure everything's being done.</t>
   </si>
   <si>
@@ -87,14 +81,37 @@
   </si>
   <si>
     <t>see m_functionAdd_Type_Event</t>
+  </si>
+  <si>
+    <t>Save project to DB</t>
+  </si>
+  <si>
+    <t>write code methods listed below</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -122,14 +139,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -404,22 +451,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -427,7 +474,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -435,85 +482,85 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="A19" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>19</v>
-      </c>
-      <c r="E22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
In code.js: did removeEvent and renameEvent.
</commit_message>
<xml_diff>
--- a/finish code.xlsx
+++ b/finish code.xlsx
@@ -454,7 +454,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -521,12 +521,12 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
In code.js: did m_functionRemove_Type_Event.
</commit_message>
<xml_diff>
--- a/finish code.xlsx
+++ b/finish code.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>remove rename Type and Method;</t>
   </si>
@@ -56,9 +56,6 @@
     <t>test</t>
   </si>
   <si>
-    <t>methods in code.js to finish</t>
-  </si>
-  <si>
     <t>self.removeEvent</t>
   </si>
   <si>
@@ -80,13 +77,13 @@
     <t>m_functionRemove_Type_Event</t>
   </si>
   <si>
-    <t>see m_functionAdd_Type_Event</t>
-  </si>
-  <si>
     <t>Save project to DB</t>
   </si>
   <si>
     <t>write code methods listed below</t>
+  </si>
+  <si>
+    <t>methods in code.js to test</t>
   </si>
 </sst>
 </file>
@@ -451,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -486,8 +483,11 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -517,50 +517,47 @@
     </row>
     <row r="15" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+    <row r="20" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>17</v>
-      </c>
-      <c r="E18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All ready to change generation of blocks and javaScript in code.js. SS
</commit_message>
<xml_diff>
--- a/finish code.xlsx
+++ b/finish code.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>remove rename Type and Method;</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Saturday</t>
   </si>
   <si>
-    <t>Sunday</t>
-  </si>
-  <si>
-    <t>Monday</t>
-  </si>
-  <si>
     <t>test TI rename</t>
   </si>
   <si>
@@ -84,6 +78,18 @@
   </si>
   <si>
     <t>methods in code.js to test</t>
+  </si>
+  <si>
+    <t>in m_functionGenerateBlocksTypeNewFunctionString and m_functionGenerateJavaScriptTypeNewFunctionString</t>
+  </si>
+  <si>
+    <t>in m_functionGenerateBlocksMethodFunctionString and m_functionGenerateJavaScriptMethodFunctionString</t>
+  </si>
+  <si>
+    <t>Sunday-Monday</t>
+  </si>
+  <si>
+    <t>After Monday</t>
   </si>
 </sst>
 </file>
@@ -448,20 +454,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -469,7 +478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -477,87 +486,97 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+    <row r="21" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B22" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>